<commit_message>
- test case added.
</commit_message>
<xml_diff>
--- a/Tests/Test Cases/community.xlsx
+++ b/Tests/Test Cases/community.xlsx
@@ -5,11 +5,11 @@
   <workbookPr filterPrivacy="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tthakgunduz/Desktop/SWE574/GiTHUB/docs-repo/Tests/Test Cases/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tthakgunduz/Desktop/ALL/Master-BOUN/SWE574/GiTHUB/docs-repo/Tests/Test Cases/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-40" yWindow="3340" windowWidth="24000" windowHeight="13560"/>
+    <workbookView xWindow="-200" yWindow="2020" windowWidth="28800" windowHeight="17460"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Task Name</t>
   </si>
@@ -60,6 +60,89 @@
   </si>
   <si>
     <t xml:space="preserve">#186, </t>
+  </si>
+  <si>
+    <t>1-Open http://localhost:8080/index.html
+2-Login with username emre.gurer@gmail.com and password 123.
+3-Click on details of Web Sustainability Community</t>
+  </si>
+  <si>
+    <t>User views details of a topic.</t>
+  </si>
+  <si>
+    <t>1- Click on "Sustainable Web Design Resource" topic.</t>
+  </si>
+  <si>
+    <t>Topic details with comments and resources are listed.</t>
+  </si>
+  <si>
+    <t>User returns to community detail page.</t>
+  </si>
+  <si>
+    <t>1- Click on return to community on topic detail page.</t>
+  </si>
+  <si>
+    <t>"Web Sustainability" community's detail page is opened.</t>
+  </si>
+  <si>
+    <t>User views member profile.</t>
+  </si>
+  <si>
+    <t>1- Click on İlyas Alper Karatepe text</t>
+  </si>
+  <si>
+    <t>User profile page is opened.</t>
+  </si>
+  <si>
+    <t>User views all members</t>
+  </si>
+  <si>
+    <t>1- Click on see all members</t>
+  </si>
+  <si>
+    <t>List is displayed:
+İlyas Alper Karatepe
+Emre Gürer</t>
+  </si>
+  <si>
+    <t>User views upcoming event in detail</t>
+  </si>
+  <si>
+    <t>1- Click on meeting on 21 December</t>
+  </si>
+  <si>
+    <t>Meeting page is opened.</t>
+  </si>
+  <si>
+    <t>User views resources of community</t>
+  </si>
+  <si>
+    <t>1- Click on alper.png</t>
+  </si>
+  <si>
+    <t>Image is opened</t>
+  </si>
+  <si>
+    <t>User views community requests</t>
+  </si>
+  <si>
+    <t>1- Click on community requests</t>
+  </si>
+  <si>
+    <t>No request is displayed.</t>
+  </si>
+  <si>
+    <t>User creates a topic</t>
+  </si>
+  <si>
+    <t>1- Click on create topic
+2-Title about web
+3-Description web will be explained
+4-tag web
+5-Click create</t>
+  </si>
+  <si>
+    <t>Topic is created and topic detail page is opened.</t>
   </si>
 </sst>
 </file>
@@ -555,7 +638,7 @@
   <dimension ref="A1:H71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -600,7 +683,7 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="75" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -610,7 +693,9 @@
       <c r="C3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="8"/>
+      <c r="D3" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="E3" s="8"/>
       <c r="F3" s="9" t="s">
         <v>10</v>
@@ -618,25 +703,37 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>2</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
+      <c r="B4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>13</v>
+      </c>
       <c r="E4" s="8"/>
       <c r="F4" s="9"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>3</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
+      <c r="B5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>16</v>
+      </c>
       <c r="E5" s="8"/>
       <c r="F5" s="9"/>
       <c r="G5" s="1"/>
@@ -646,21 +743,33 @@
       <c r="A6" s="3">
         <v>4</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
+      <c r="B6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>19</v>
+      </c>
       <c r="E6" s="8"/>
       <c r="F6" s="9"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>5</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
+      <c r="B7" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="E7" s="8"/>
       <c r="F7" s="9"/>
       <c r="G7" s="1"/>
@@ -670,9 +779,15 @@
       <c r="A8" s="3">
         <v>6</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
+      <c r="B8" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>25</v>
+      </c>
       <c r="E8" s="8"/>
       <c r="F8" s="9"/>
       <c r="G8" s="1"/>
@@ -682,9 +797,15 @@
       <c r="A9" s="3">
         <v>7</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
+      <c r="B9" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>28</v>
+      </c>
       <c r="E9" s="8"/>
       <c r="F9" s="9"/>
       <c r="G9" s="1"/>
@@ -694,21 +815,33 @@
       <c r="A10" s="3">
         <v>8</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
+      <c r="B10" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>31</v>
+      </c>
       <c r="E10" s="8"/>
       <c r="F10" s="9"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="75" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>9</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
+      <c r="B11" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>34</v>
+      </c>
       <c r="E11" s="8"/>
       <c r="F11" s="9"/>
       <c r="G11" s="1"/>

</xml_diff>